<commit_message>
pseudotime early + late
</commit_message>
<xml_diff>
--- a/GO Heatmap HCADtrajectory early2.xlsx
+++ b/GO Heatmap HCADtrajectory early2.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://radboudumc-my.sharepoint.com/personal/felicitas_pardow_radboudumc_nl/Documents/Results/KCsinAD/FPcomp/KCinAD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="11_FDF989BC4F104A92C692C4CC96B3E370405BF8DF" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9ED1C88A-DFE0-43C0-A731-021FEF9C524E}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="11_FDF989BC4F104A92C692C4CC96B3E370405BF8DF" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{391AFACC-0BC1-4255-80FB-2C24C4DC12FD}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1065" yWindow="1455" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Early_ASS1down" sheetId="1" r:id="rId1"/>
-    <sheet name="Early_KRT15down" sheetId="2" r:id="rId2"/>
+    <sheet name="Early_C1,2down" sheetId="1" r:id="rId1"/>
+    <sheet name="Early_C4,5down" sheetId="2" r:id="rId2"/>
     <sheet name="Early_nochange" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -1714,10 +1714,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2017,12 +2018,14 @@
   <dimension ref="A1:J114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="78.140625" customWidth="1"/>
+    <col min="4" max="6" width="0" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="0" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="58.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2065,7 +2068,7 @@
       <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
@@ -2289,7 +2292,7 @@
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D9" t="s">
@@ -5594,7 +5597,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6483,7 +6486,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>